<commit_message>
Preprocess for excels added
</commit_message>
<xml_diff>
--- a/excel graph/graficos barras.xlsx
+++ b/excel graph/graficos barras.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17340" yWindow="10580" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="3020" yWindow="460" windowWidth="23840" windowHeight="24420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -407,7 +407,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D8:D9"/>
+      <selection activeCell="D1" sqref="D1:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -486,7 +486,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>